<commit_message>
Added Unit SqFt column and named helper column
</commit_message>
<xml_diff>
--- a/rx_PSC_RentalActivity_v2.xlsx
+++ b/rx_PSC_RentalActivity_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BerilP\repos\PSC-RentalActivity-YSR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B41B22B-7D24-4A89-8163-4FCAD452E9F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0320DDA6-71F6-41B8-82F5-ED1BB54DBDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2730" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Rental Activity</t>
   </si>
@@ -146,15 +146,6 @@
     <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, I5:I{-1})</t>
   </si>
   <si>
-    <t>&amp;=&amp;=SUMIF(B5:B{-1},1, J5:J{-1})</t>
-  </si>
-  <si>
-    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, K5:K{-1})</t>
-  </si>
-  <si>
-    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, L5:L{-1})</t>
-  </si>
-  <si>
     <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, M5:M{-1})</t>
   </si>
   <si>
@@ -182,7 +173,28 @@
     <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, N5:N{-1})</t>
   </si>
   <si>
-    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, O5:O{-1})/SUM(B5:B{-1})</t>
+    <t>&amp;=display.UnitArea</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, J5:J{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, O5:O{-1})</t>
+  </si>
+  <si>
+    <t>Sq. Ft.</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, K5:K{-1})/SUM(B5:B{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1},1, L5:L{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, P5:P{-1})</t>
+  </si>
+  <si>
+    <t>Count of Distinct Unit Types</t>
   </si>
 </sst>
 </file>
@@ -304,14 +316,14 @@
     </xf>
     <xf numFmtId="2" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,97 +641,102 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="B4" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.26953125" customWidth="1"/>
-    <col min="2" max="2" width="23.36328125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="88.08984375" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="7.7265625" customWidth="1"/>
     <col min="4" max="4" width="9.08984375" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" customWidth="1"/>
-    <col min="6" max="6" width="8.453125" customWidth="1"/>
-    <col min="7" max="7" width="9.7265625" customWidth="1"/>
-    <col min="8" max="8" width="7.54296875" customWidth="1"/>
-    <col min="9" max="9" width="7.81640625" customWidth="1"/>
-    <col min="10" max="10" width="12.7265625" customWidth="1"/>
-    <col min="11" max="11" width="7.54296875" customWidth="1"/>
-    <col min="12" max="12" width="9.453125" customWidth="1"/>
-    <col min="13" max="13" width="12.7265625" customWidth="1"/>
-    <col min="14" max="14" width="9.26953125" customWidth="1"/>
-    <col min="15" max="15" width="6.26953125" customWidth="1"/>
-    <col min="16" max="16" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.453125" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" customWidth="1"/>
+    <col min="8" max="8" width="9.7265625" customWidth="1"/>
+    <col min="9" max="9" width="7.54296875" customWidth="1"/>
+    <col min="10" max="11" width="7.81640625" customWidth="1"/>
+    <col min="12" max="12" width="12.7265625" customWidth="1"/>
+    <col min="13" max="13" width="7.54296875" customWidth="1"/>
+    <col min="14" max="14" width="9.453125" customWidth="1"/>
+    <col min="15" max="15" width="12.7265625" customWidth="1"/>
+    <col min="16" max="16" width="9.26953125" customWidth="1"/>
+    <col min="17" max="17" width="21.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
     </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
     </row>
-    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
@@ -727,43 +744,46 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="K4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="M4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -777,49 +797,52 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="M5" s="5" t="s">
+      <c r="N5" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="O5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="P5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="P5" s="2" t="s">
+      <c r="Q5" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>30</v>
@@ -840,35 +863,38 @@
         <v>35</v>
       </c>
       <c r="J6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="N6" s="6" t="s">
+      <c r="N6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="O6" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="O6" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="P6" s="3"/>
+      <c r="P6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q6" s="3"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" t="s">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A2:P2"/>
-    <mergeCell ref="A3:P3"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A2:Q2"/>
+    <mergeCell ref="A3:Q3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.7" bottom="0.7" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="990" orientation="portrait" useFirstPageNumber="1"/>
@@ -880,7 +906,7 @@
     <brk id="29" max="16383" man="1"/>
   </rowBreaks>
   <ignoredErrors>
-    <ignoredError sqref="C4:D4 A1 A4 M4:O4 F4:I4" numberStoredAsText="1"/>
+    <ignoredError sqref="C4:D4 A1 A4 O4:P4 G4:J4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding files for summary level report
</commit_message>
<xml_diff>
--- a/rx_PSC_RentalActivity_v2.xlsx
+++ b/rx_PSC_RentalActivity_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BerilP\repos\PSC-RentalActivity-YSR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0320DDA6-71F6-41B8-82F5-ED1BB54DBDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97114894-DCC0-4DF2-8B64-F035D065013A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2730" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -644,7 +644,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B4" sqref="B1:B1048576"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Sq Ft % and Sq Ft Change %
</commit_message>
<xml_diff>
--- a/rx_PSC_RentalActivity_v2.xlsx
+++ b/rx_PSC_RentalActivity_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BerilP\repos\PSC-RentalActivity-YSR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97114894-DCC0-4DF2-8B64-F035D065013A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E43F3D2-37C5-407A-832A-880F059BC71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2730" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PS" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Rental Activity</t>
   </si>
@@ -56,15 +56,6 @@
     <t>Move Outs</t>
   </si>
   <si>
-    <t>Net Occ.</t>
-  </si>
-  <si>
-    <t>End Occ.</t>
-  </si>
-  <si>
-    <t>Occupied Area</t>
-  </si>
-  <si>
     <t>Total Area</t>
   </si>
   <si>
@@ -155,9 +146,6 @@
     <t>&amp;=header.Property</t>
   </si>
   <si>
-    <t>Begin Occ.</t>
-  </si>
-  <si>
     <t>Vacant</t>
   </si>
   <si>
@@ -170,31 +158,55 @@
     <t>Future Resrv.</t>
   </si>
   <si>
-    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, N5:N{-1})</t>
-  </si>
-  <si>
     <t>&amp;=display.UnitArea</t>
   </si>
   <si>
     <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, J5:J{-1})</t>
   </si>
   <si>
-    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, O5:O{-1})</t>
-  </si>
-  <si>
     <t>Sq. Ft.</t>
   </si>
   <si>
-    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, K5:K{-1})/SUM(B5:B{-1})</t>
-  </si>
-  <si>
-    <t>&amp;=&amp;=SUMIF(B5:B{-1},1, L5:L{-1})</t>
-  </si>
-  <si>
     <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, P5:P{-1})</t>
   </si>
   <si>
     <t>Count of Distinct Unit Types</t>
+  </si>
+  <si>
+    <t>Occ. Change</t>
+  </si>
+  <si>
+    <t>Tot Rented</t>
+  </si>
+  <si>
+    <t>Occupied Sq Ft</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, K5:K{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, L5:L{-1})/SUM(B5:B{-1})</t>
+  </si>
+  <si>
+    <t>Begin</t>
+  </si>
+  <si>
+    <t>Sq Ft %</t>
+  </si>
+  <si>
+    <t>&amp;=display.OccSqFt</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1},1, O5:O{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, Q5:Q{-1})</t>
+  </si>
+  <si>
+    <t>Sq Ft Change %</t>
+  </si>
+  <si>
+    <t>&amp;=display.SqFtChange</t>
   </si>
 </sst>
 </file>
@@ -303,12 +315,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -318,6 +328,18 @@
     <xf numFmtId="2" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -641,260 +663,277 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.26953125" customWidth="1"/>
     <col min="2" max="2" width="88.08984375" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7265625" customWidth="1"/>
-    <col min="4" max="4" width="9.08984375" customWidth="1"/>
-    <col min="5" max="5" width="7.453125" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" customWidth="1"/>
-    <col min="7" max="7" width="8.453125" customWidth="1"/>
-    <col min="8" max="8" width="9.7265625" customWidth="1"/>
-    <col min="9" max="9" width="7.54296875" customWidth="1"/>
-    <col min="10" max="11" width="7.81640625" customWidth="1"/>
-    <col min="12" max="12" width="12.7265625" customWidth="1"/>
-    <col min="13" max="13" width="7.54296875" customWidth="1"/>
-    <col min="14" max="14" width="9.453125" customWidth="1"/>
-    <col min="15" max="15" width="12.7265625" customWidth="1"/>
-    <col min="16" max="16" width="9.26953125" customWidth="1"/>
-    <col min="17" max="17" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.7265625" customWidth="1"/>
+    <col min="5" max="6" width="9.08984375" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" customWidth="1"/>
+    <col min="8" max="8" width="8.453125" customWidth="1"/>
+    <col min="9" max="9" width="9.7265625" customWidth="1"/>
+    <col min="10" max="10" width="7.54296875" customWidth="1"/>
+    <col min="11" max="15" width="7.81640625" customWidth="1"/>
+    <col min="16" max="16" width="12.7265625" customWidth="1"/>
+    <col min="17" max="17" width="7.54296875" customWidth="1"/>
+    <col min="18" max="18" width="9.453125" customWidth="1"/>
+    <col min="19" max="19" width="21.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+    </row>
+    <row r="4" spans="1:19" s="13" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="S4" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
+      <c r="S5" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
+    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="S6" s="2"/>
     </row>
-    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q4" s="4" t="s">
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="N6" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q6" s="3"/>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G17" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="A2:Q2"/>
-    <mergeCell ref="A3:Q3"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A2:S2"/>
+    <mergeCell ref="A3:S3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.7" bottom="0.7" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="990" orientation="portrait" useFirstPageNumber="1"/>
@@ -906,7 +945,7 @@
     <brk id="29" max="16383" man="1"/>
   </rowBreaks>
   <ignoredErrors>
-    <ignoredError sqref="C4:D4 A1 A4 O4:P4 G4:J4" numberStoredAsText="1"/>
+    <ignoredError sqref="E4 A1 A4 H4:I4 C4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>